<commit_message>
Lap Realisasi, SPTJ, SPTMH Fix
Fix:
Lap Realisasi
SPTJ
SPTMH

WIP:
K7 Kab (trouble di saldo)
</commit_message>
<xml_diff>
--- a/format/k7_kab1.xlsx
+++ b/format/k7_kab1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\amanbos\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A782A1DC-8805-4427-B173-EC8EB3CB9F80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA39EE44-A064-4A9B-B68D-3DDED3F443FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2806AC20-E28C-4D3D-8610-2A31688B425C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2806AC20-E28C-4D3D-8610-2A31688B425C}"/>
   </bookViews>
   <sheets>
     <sheet name="K7 TW 3 KAB" sheetId="1" r:id="rId1"/>
@@ -801,12 +801,168 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,176 +998,13 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1065,7 +1058,7 @@
       <sheetName val="data NPSN"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="4">
           <cell r="B4">
@@ -1090,17 +1083,6 @@
         </row>
       </sheetData>
       <sheetData sheetId="2">
-        <row r="11">
-          <cell r="C11" t="str">
-            <v>Juli</v>
-          </cell>
-          <cell r="E11">
-            <v>100</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>(1.01) Honorarium Pengelola Keuangan</v>
-          </cell>
-        </row>
         <row r="60">
           <cell r="R60" t="str">
             <v>(3.01) Belanja Modal Mesin dan Peralatan</v>
@@ -1129,15 +1111,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1447,17 +1429,17 @@
   <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="4" customWidth="1"/>
-    <col min="2" max="9" width="14.26953125" style="4"/>
-    <col min="10" max="10" width="4.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
+    <col min="2" max="9" width="14.21875" style="4"/>
+    <col min="10" max="10" width="4.77734375" style="4" customWidth="1"/>
     <col min="11" max="11" width="5" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="19.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="14.26953125" style="4"/>
+    <col min="12" max="12" width="19.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="14.21875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1472,177 +1454,177 @@
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
+      <c r="B2" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="8">
+      <c r="B4" s="60">
         <f>[1]REKAPITULASI!B4</f>
         <v>20320774</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="str">
+      <c r="C4" s="61"/>
+      <c r="D4" s="62" t="str">
         <f>[1]REKAPITULASI!C4</f>
         <v>SD NEGERI BATUR 01</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13" t="str">
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="65" t="str">
         <f>[1]REKAPITULASI!F4</f>
         <v>GETASAN</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17">
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="69">
         <f>[1]CEK!C5</f>
         <v>11650000</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22">
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49">
         <f>[1]CEK!C6</f>
         <v>12640000</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27">
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="7">
         <f>F10+F15+F61</f>
         <v>0</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="7">
         <f t="shared" ref="G8:H8" si="0">G10+G15+G61</f>
         <v>0</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="8">
         <f>SUM(F8:H8)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36">
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="11">
         <f>SUM(F11:F14)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="11">
         <f t="shared" ref="G10:I10" si="1">SUM(G11:G14)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="7"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="41">
-        <v>0</v>
-      </c>
-      <c r="G11" s="41">
-        <v>0</v>
-      </c>
-      <c r="H11" s="41">
-        <v>0</v>
-      </c>
-      <c r="I11" s="42">
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
         <f>SUM(F11:H11)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="4" t="str">
         <f>RIGHT(I11,2)</f>
         <v>0</v>
@@ -1654,26 +1636,26 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="41">
-        <v>0</v>
-      </c>
-      <c r="G12" s="41">
-        <v>0</v>
-      </c>
-      <c r="H12" s="41">
-        <v>0</v>
-      </c>
-      <c r="I12" s="42">
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
         <f>SUM(F12:H12)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="7"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="4" t="str">
         <f t="shared" ref="K12:K29" si="2">RIGHT(I12,2)</f>
         <v>0</v>
@@ -1685,26 +1667,26 @@
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="41">
-        <v>0</v>
-      </c>
-      <c r="G13" s="41">
-        <v>0</v>
-      </c>
-      <c r="H13" s="41">
-        <v>0</v>
-      </c>
-      <c r="I13" s="42">
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
         <f>SUM(F13:H13)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="6"/>
       <c r="K13" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1716,26 +1698,26 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="41">
-        <v>0</v>
-      </c>
-      <c r="G14" s="41">
-        <v>0</v>
-      </c>
-      <c r="H14" s="41">
-        <v>0</v>
-      </c>
-      <c r="I14" s="42">
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
         <f>SUM(F14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="7"/>
+      <c r="J14" s="6"/>
       <c r="K14" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1745,54 +1727,54 @@
         <v>.</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="36">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="11">
         <f>SUM(F16:F60)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="11">
         <f t="shared" ref="G15:I15" si="4">SUM(G16:G60)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="12">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="41">
-        <v>0</v>
-      </c>
-      <c r="G16" s="41">
-        <v>0</v>
-      </c>
-      <c r="H16" s="41">
-        <v>0</v>
-      </c>
-      <c r="I16" s="42">
+      <c r="F16" s="16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
         <f t="shared" ref="I16:I60" si="5">SUM(F16:H16)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="6"/>
       <c r="K16" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1804,26 +1786,26 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="41">
-        <v>0</v>
-      </c>
-      <c r="G17" s="41">
-        <v>0</v>
-      </c>
-      <c r="H17" s="41">
-        <v>0</v>
-      </c>
-      <c r="I17" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="7"/>
+      <c r="F17" s="16">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="6"/>
       <c r="K17" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1835,26 +1817,26 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="41">
-        <v>0</v>
-      </c>
-      <c r="G18" s="41">
-        <v>0</v>
-      </c>
-      <c r="H18" s="41">
-        <v>0</v>
-      </c>
-      <c r="I18" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="7"/>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0</v>
+      </c>
+      <c r="I18" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="6"/>
       <c r="K18" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1866,26 +1848,26 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="47" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="41">
-        <v>0</v>
-      </c>
-      <c r="G19" s="41">
-        <v>0</v>
-      </c>
-      <c r="H19" s="41">
-        <v>0</v>
-      </c>
-      <c r="I19" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="7"/>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0</v>
+      </c>
+      <c r="H19" s="16">
+        <v>0</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="6"/>
       <c r="K19" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1897,26 +1879,26 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="47" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="41">
-        <v>0</v>
-      </c>
-      <c r="G20" s="41">
-        <v>0</v>
-      </c>
-      <c r="H20" s="41">
-        <v>0</v>
-      </c>
-      <c r="I20" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="7"/>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0</v>
+      </c>
+      <c r="H20" s="16">
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="6"/>
       <c r="K20" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1928,26 +1910,26 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="47" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="41">
-        <v>0</v>
-      </c>
-      <c r="G21" s="41">
-        <v>0</v>
-      </c>
-      <c r="H21" s="41">
-        <v>0</v>
-      </c>
-      <c r="I21" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="7"/>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="6"/>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1959,26 +1941,26 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="41">
-        <v>0</v>
-      </c>
-      <c r="G22" s="41">
-        <v>0</v>
-      </c>
-      <c r="H22" s="41">
-        <v>0</v>
-      </c>
-      <c r="I22" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="7"/>
+      <c r="F22" s="16">
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="6"/>
       <c r="K22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1990,26 +1972,26 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="47" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="41">
-        <v>0</v>
-      </c>
-      <c r="G23" s="41">
-        <v>0</v>
-      </c>
-      <c r="H23" s="41">
-        <v>0</v>
-      </c>
-      <c r="I23" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="7"/>
+      <c r="F23" s="16">
+        <v>0</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="6"/>
       <c r="K23" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2021,26 +2003,26 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="47" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="41">
-        <v>0</v>
-      </c>
-      <c r="G24" s="41">
-        <v>0</v>
-      </c>
-      <c r="H24" s="41">
-        <v>0</v>
-      </c>
-      <c r="I24" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="7"/>
+      <c r="F24" s="16">
+        <v>0</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+      <c r="I24" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="6"/>
       <c r="K24" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2052,26 +2034,26 @@
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="47" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="41">
-        <v>0</v>
-      </c>
-      <c r="G25" s="41">
-        <v>0</v>
-      </c>
-      <c r="H25" s="41">
-        <v>0</v>
-      </c>
-      <c r="I25" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="7"/>
+      <c r="F25" s="16">
+        <v>0</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+      <c r="I25" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="6"/>
       <c r="K25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2083,26 +2065,26 @@
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="41">
-        <v>0</v>
-      </c>
-      <c r="G26" s="41">
-        <v>0</v>
-      </c>
-      <c r="H26" s="41">
-        <v>0</v>
-      </c>
-      <c r="I26" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="7"/>
+      <c r="F26" s="16">
+        <v>0</v>
+      </c>
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="6"/>
       <c r="K26" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2114,26 +2096,26 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="47" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="41">
-        <v>0</v>
-      </c>
-      <c r="G27" s="41">
-        <v>0</v>
-      </c>
-      <c r="H27" s="41">
-        <v>0</v>
-      </c>
-      <c r="I27" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="7"/>
+      <c r="F27" s="16">
+        <v>0</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="6"/>
       <c r="K27" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2145,26 +2127,26 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="47" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="41">
-        <v>0</v>
-      </c>
-      <c r="G28" s="41">
-        <v>0</v>
-      </c>
-      <c r="H28" s="41">
-        <v>0</v>
-      </c>
-      <c r="I28" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="7"/>
+      <c r="F28" s="16">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="6"/>
       <c r="K28" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2176,26 +2158,26 @@
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="47" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="41">
-        <v>0</v>
-      </c>
-      <c r="G29" s="41">
-        <v>0</v>
-      </c>
-      <c r="H29" s="41">
-        <v>0</v>
-      </c>
-      <c r="I29" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="7"/>
+      <c r="F29" s="16">
+        <v>0</v>
+      </c>
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="6"/>
       <c r="K29" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2207,95 +2189,95 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="47" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="41">
-        <v>0</v>
-      </c>
-      <c r="G30" s="41">
-        <v>0</v>
-      </c>
-      <c r="H30" s="41">
-        <v>0</v>
-      </c>
-      <c r="I30" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="7"/>
+      <c r="F30" s="16">
+        <v>0</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0</v>
+      </c>
+      <c r="I30" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="47" t="s">
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="41">
-        <v>0</v>
-      </c>
-      <c r="G31" s="41">
-        <v>0</v>
-      </c>
-      <c r="H31" s="41">
-        <v>0</v>
-      </c>
-      <c r="I31" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="7"/>
+      <c r="F31" s="16">
+        <v>0</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0</v>
+      </c>
+      <c r="H31" s="16">
+        <v>0</v>
+      </c>
+      <c r="I31" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="47" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="41">
-        <v>0</v>
-      </c>
-      <c r="G32" s="41">
-        <v>0</v>
-      </c>
-      <c r="H32" s="41">
-        <v>0</v>
-      </c>
-      <c r="I32" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="7"/>
+      <c r="F32" s="16">
+        <v>0</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0</v>
+      </c>
+      <c r="H32" s="16">
+        <v>0</v>
+      </c>
+      <c r="I32" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="47" t="s">
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="41">
-        <v>0</v>
-      </c>
-      <c r="G33" s="41">
-        <v>0</v>
-      </c>
-      <c r="H33" s="41">
-        <v>0</v>
-      </c>
-      <c r="I33" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="7"/>
+      <c r="F33" s="16">
+        <v>0</v>
+      </c>
+      <c r="G33" s="16">
+        <v>0</v>
+      </c>
+      <c r="H33" s="16">
+        <v>0</v>
+      </c>
+      <c r="I33" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="6"/>
       <c r="K33" s="4" t="str">
         <f t="shared" ref="K33:K64" si="6">RIGHT(I33,2)</f>
         <v>0</v>
@@ -2307,26 +2289,26 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="47" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="41">
-        <v>0</v>
-      </c>
-      <c r="G34" s="41">
-        <v>0</v>
-      </c>
-      <c r="H34" s="41">
-        <v>0</v>
-      </c>
-      <c r="I34" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="7"/>
+      <c r="F34" s="16">
+        <v>0</v>
+      </c>
+      <c r="G34" s="16">
+        <v>0</v>
+      </c>
+      <c r="H34" s="16">
+        <v>0</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="6"/>
       <c r="K34" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2334,26 +2316,26 @@
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="47" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="41">
-        <v>0</v>
-      </c>
-      <c r="G35" s="41">
-        <v>0</v>
-      </c>
-      <c r="H35" s="41">
-        <v>0</v>
-      </c>
-      <c r="I35" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="7"/>
+      <c r="F35" s="16">
+        <v>0</v>
+      </c>
+      <c r="G35" s="16">
+        <v>0</v>
+      </c>
+      <c r="H35" s="16">
+        <v>0</v>
+      </c>
+      <c r="I35" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="6"/>
       <c r="K35" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2365,26 +2347,26 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="47" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="41">
-        <v>0</v>
-      </c>
-      <c r="G36" s="41">
-        <v>0</v>
-      </c>
-      <c r="H36" s="41">
-        <v>0</v>
-      </c>
-      <c r="I36" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="7"/>
+      <c r="F36" s="16">
+        <v>0</v>
+      </c>
+      <c r="G36" s="16">
+        <v>0</v>
+      </c>
+      <c r="H36" s="16">
+        <v>0</v>
+      </c>
+      <c r="I36" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="6"/>
       <c r="K36" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2396,26 +2378,26 @@
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="47" t="s">
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="41">
-        <v>0</v>
-      </c>
-      <c r="G37" s="41">
-        <v>0</v>
-      </c>
-      <c r="H37" s="41">
-        <v>0</v>
-      </c>
-      <c r="I37" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="7"/>
+      <c r="F37" s="16">
+        <v>0</v>
+      </c>
+      <c r="G37" s="16">
+        <v>0</v>
+      </c>
+      <c r="H37" s="16">
+        <v>0</v>
+      </c>
+      <c r="I37" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="6"/>
       <c r="K37" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2427,26 +2409,26 @@
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="47" t="s">
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="41">
-        <v>0</v>
-      </c>
-      <c r="G38" s="41">
-        <v>0</v>
-      </c>
-      <c r="H38" s="41">
-        <v>0</v>
-      </c>
-      <c r="I38" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="7"/>
+      <c r="F38" s="16">
+        <v>0</v>
+      </c>
+      <c r="G38" s="16">
+        <v>0</v>
+      </c>
+      <c r="H38" s="16">
+        <v>0</v>
+      </c>
+      <c r="I38" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="6"/>
       <c r="K38" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2458,26 +2440,26 @@
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="47" t="s">
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="41">
-        <v>0</v>
-      </c>
-      <c r="G39" s="41">
-        <v>0</v>
-      </c>
-      <c r="H39" s="41">
-        <v>0</v>
-      </c>
-      <c r="I39" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="7"/>
+      <c r="F39" s="16">
+        <v>0</v>
+      </c>
+      <c r="G39" s="16">
+        <v>0</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="6"/>
       <c r="K39" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2489,26 +2471,26 @@
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="47" t="s">
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="41">
-        <v>0</v>
-      </c>
-      <c r="G40" s="41">
-        <v>0</v>
-      </c>
-      <c r="H40" s="41">
-        <v>0</v>
-      </c>
-      <c r="I40" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="7"/>
+      <c r="F40" s="16">
+        <v>0</v>
+      </c>
+      <c r="G40" s="16">
+        <v>0</v>
+      </c>
+      <c r="H40" s="16">
+        <v>0</v>
+      </c>
+      <c r="I40" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="6"/>
       <c r="K40" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2520,26 +2502,26 @@
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="47" t="s">
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="41">
-        <v>0</v>
-      </c>
-      <c r="G41" s="41">
-        <v>0</v>
-      </c>
-      <c r="H41" s="41">
-        <v>0</v>
-      </c>
-      <c r="I41" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J41" s="7"/>
+      <c r="F41" s="16">
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <v>0</v>
+      </c>
+      <c r="H41" s="16">
+        <v>0</v>
+      </c>
+      <c r="I41" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="6"/>
       <c r="K41" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2551,26 +2533,26 @@
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="47" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="41">
-        <v>0</v>
-      </c>
-      <c r="G42" s="41">
-        <v>0</v>
-      </c>
-      <c r="H42" s="41">
-        <v>0</v>
-      </c>
-      <c r="I42" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J42" s="7"/>
+      <c r="F42" s="16">
+        <v>0</v>
+      </c>
+      <c r="G42" s="16">
+        <v>0</v>
+      </c>
+      <c r="H42" s="16">
+        <v>0</v>
+      </c>
+      <c r="I42" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="6"/>
       <c r="K42" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2582,26 +2564,26 @@
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="47" t="s">
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="41">
-        <v>0</v>
-      </c>
-      <c r="G43" s="41">
-        <v>0</v>
-      </c>
-      <c r="H43" s="41">
-        <v>0</v>
-      </c>
-      <c r="I43" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J43" s="7"/>
+      <c r="F43" s="16">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16">
+        <v>0</v>
+      </c>
+      <c r="H43" s="16">
+        <v>0</v>
+      </c>
+      <c r="I43" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="6"/>
       <c r="K43" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2613,26 +2595,26 @@
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="47" t="s">
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="41">
-        <v>0</v>
-      </c>
-      <c r="G44" s="41">
-        <v>0</v>
-      </c>
-      <c r="H44" s="41">
-        <v>0</v>
-      </c>
-      <c r="I44" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="7"/>
+      <c r="F44" s="16">
+        <v>0</v>
+      </c>
+      <c r="G44" s="16">
+        <v>0</v>
+      </c>
+      <c r="H44" s="16">
+        <v>0</v>
+      </c>
+      <c r="I44" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="6"/>
       <c r="K44" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2644,26 +2626,26 @@
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="47" t="s">
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="41">
-        <v>0</v>
-      </c>
-      <c r="G45" s="41">
-        <v>0</v>
-      </c>
-      <c r="H45" s="41">
-        <v>0</v>
-      </c>
-      <c r="I45" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="7"/>
+      <c r="F45" s="16">
+        <v>0</v>
+      </c>
+      <c r="G45" s="16">
+        <v>0</v>
+      </c>
+      <c r="H45" s="16">
+        <v>0</v>
+      </c>
+      <c r="I45" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="6"/>
       <c r="K45" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2675,26 +2657,26 @@
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="47" t="s">
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="41">
-        <v>0</v>
-      </c>
-      <c r="G46" s="41">
-        <v>0</v>
-      </c>
-      <c r="H46" s="41">
-        <v>0</v>
-      </c>
-      <c r="I46" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J46" s="7"/>
+      <c r="F46" s="16">
+        <v>0</v>
+      </c>
+      <c r="G46" s="16">
+        <v>0</v>
+      </c>
+      <c r="H46" s="16">
+        <v>0</v>
+      </c>
+      <c r="I46" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="6"/>
       <c r="K46" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2706,26 +2688,26 @@
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="47" t="s">
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="41">
-        <v>0</v>
-      </c>
-      <c r="G47" s="41">
-        <v>0</v>
-      </c>
-      <c r="H47" s="41">
-        <v>0</v>
-      </c>
-      <c r="I47" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J47" s="7"/>
+      <c r="F47" s="16">
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <v>0</v>
+      </c>
+      <c r="H47" s="16">
+        <v>0</v>
+      </c>
+      <c r="I47" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="6"/>
       <c r="K47" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2737,26 +2719,26 @@
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="47" t="s">
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="41">
-        <v>0</v>
-      </c>
-      <c r="G48" s="41">
-        <v>0</v>
-      </c>
-      <c r="H48" s="41">
-        <v>0</v>
-      </c>
-      <c r="I48" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="7"/>
+      <c r="F48" s="16">
+        <v>0</v>
+      </c>
+      <c r="G48" s="16">
+        <v>0</v>
+      </c>
+      <c r="H48" s="16">
+        <v>0</v>
+      </c>
+      <c r="I48" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="6"/>
       <c r="K48" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2768,26 +2750,26 @@
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="47" t="s">
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F49" s="41">
-        <v>0</v>
-      </c>
-      <c r="G49" s="41">
-        <v>0</v>
-      </c>
-      <c r="H49" s="41">
-        <v>0</v>
-      </c>
-      <c r="I49" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J49" s="7"/>
+      <c r="F49" s="16">
+        <v>0</v>
+      </c>
+      <c r="G49" s="16">
+        <v>0</v>
+      </c>
+      <c r="H49" s="16">
+        <v>0</v>
+      </c>
+      <c r="I49" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="6"/>
       <c r="K49" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2799,26 +2781,26 @@
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="47" t="s">
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F50" s="41">
-        <v>0</v>
-      </c>
-      <c r="G50" s="41">
-        <v>0</v>
-      </c>
-      <c r="H50" s="41">
-        <v>0</v>
-      </c>
-      <c r="I50" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J50" s="7"/>
+      <c r="F50" s="16">
+        <v>0</v>
+      </c>
+      <c r="G50" s="16">
+        <v>0</v>
+      </c>
+      <c r="H50" s="16">
+        <v>0</v>
+      </c>
+      <c r="I50" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="6"/>
       <c r="K50" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2830,26 +2812,26 @@
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="47" t="s">
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="41">
-        <v>0</v>
-      </c>
-      <c r="G51" s="41">
-        <v>0</v>
-      </c>
-      <c r="H51" s="41">
-        <v>0</v>
-      </c>
-      <c r="I51" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J51" s="7"/>
+      <c r="F51" s="16">
+        <v>0</v>
+      </c>
+      <c r="G51" s="16">
+        <v>0</v>
+      </c>
+      <c r="H51" s="16">
+        <v>0</v>
+      </c>
+      <c r="I51" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="6"/>
       <c r="K51" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2861,26 +2843,26 @@
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="47" t="s">
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F52" s="41">
-        <v>0</v>
-      </c>
-      <c r="G52" s="41">
-        <v>0</v>
-      </c>
-      <c r="H52" s="41">
-        <v>0</v>
-      </c>
-      <c r="I52" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J52" s="7"/>
+      <c r="F52" s="16">
+        <v>0</v>
+      </c>
+      <c r="G52" s="16">
+        <v>0</v>
+      </c>
+      <c r="H52" s="16">
+        <v>0</v>
+      </c>
+      <c r="I52" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="6"/>
       <c r="K52" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2892,26 +2874,26 @@
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="47" t="s">
+      <c r="B53" s="18"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F53" s="41">
-        <v>0</v>
-      </c>
-      <c r="G53" s="41">
-        <v>0</v>
-      </c>
-      <c r="H53" s="41">
-        <v>0</v>
-      </c>
-      <c r="I53" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J53" s="7"/>
+      <c r="F53" s="16">
+        <v>0</v>
+      </c>
+      <c r="G53" s="16">
+        <v>0</v>
+      </c>
+      <c r="H53" s="16">
+        <v>0</v>
+      </c>
+      <c r="I53" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="6"/>
       <c r="K53" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2923,26 +2905,26 @@
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="47" t="s">
+      <c r="B54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="41">
-        <v>0</v>
-      </c>
-      <c r="G54" s="41">
-        <v>0</v>
-      </c>
-      <c r="H54" s="41">
-        <v>0</v>
-      </c>
-      <c r="I54" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="7"/>
+      <c r="F54" s="16">
+        <v>0</v>
+      </c>
+      <c r="G54" s="16">
+        <v>0</v>
+      </c>
+      <c r="H54" s="16">
+        <v>0</v>
+      </c>
+      <c r="I54" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="6"/>
       <c r="K54" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2954,26 +2936,26 @@
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="47" t="s">
+      <c r="B55" s="18"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="41">
-        <v>0</v>
-      </c>
-      <c r="G55" s="41">
-        <v>0</v>
-      </c>
-      <c r="H55" s="41">
-        <v>0</v>
-      </c>
-      <c r="I55" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="7"/>
+      <c r="F55" s="16">
+        <v>0</v>
+      </c>
+      <c r="G55" s="16">
+        <v>0</v>
+      </c>
+      <c r="H55" s="16">
+        <v>0</v>
+      </c>
+      <c r="I55" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="6"/>
       <c r="K55" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2985,26 +2967,26 @@
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="47" t="s">
+      <c r="B56" s="18"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="41">
-        <v>0</v>
-      </c>
-      <c r="G56" s="41">
-        <v>0</v>
-      </c>
-      <c r="H56" s="41">
-        <v>0</v>
-      </c>
-      <c r="I56" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J56" s="7"/>
+      <c r="F56" s="16">
+        <v>0</v>
+      </c>
+      <c r="G56" s="16">
+        <v>0</v>
+      </c>
+      <c r="H56" s="16">
+        <v>0</v>
+      </c>
+      <c r="I56" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="6"/>
       <c r="K56" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3016,26 +2998,26 @@
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="47" t="s">
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F57" s="41">
-        <v>0</v>
-      </c>
-      <c r="G57" s="41">
-        <v>0</v>
-      </c>
-      <c r="H57" s="41">
-        <v>0</v>
-      </c>
-      <c r="I57" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="7"/>
+      <c r="F57" s="16">
+        <v>0</v>
+      </c>
+      <c r="G57" s="16">
+        <v>0</v>
+      </c>
+      <c r="H57" s="16">
+        <v>0</v>
+      </c>
+      <c r="I57" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="6"/>
       <c r="K57" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3047,26 +3029,26 @@
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="47" t="s">
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="F58" s="41">
-        <v>0</v>
-      </c>
-      <c r="G58" s="41">
-        <v>0</v>
-      </c>
-      <c r="H58" s="41">
-        <v>0</v>
-      </c>
-      <c r="I58" s="42">
+      <c r="F58" s="16">
+        <v>0</v>
+      </c>
+      <c r="G58" s="16">
+        <v>0</v>
+      </c>
+      <c r="H58" s="16">
+        <v>0</v>
+      </c>
+      <c r="I58" s="17">
         <f>SUM(F58:H58)</f>
         <v>0</v>
       </c>
-      <c r="J58" s="7"/>
+      <c r="J58" s="6"/>
       <c r="K58" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3078,26 +3060,26 @@
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="47" t="s">
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F59" s="41">
-        <v>0</v>
-      </c>
-      <c r="G59" s="41">
-        <v>0</v>
-      </c>
-      <c r="H59" s="41">
-        <v>0</v>
-      </c>
-      <c r="I59" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J59" s="7"/>
+      <c r="F59" s="16">
+        <v>0</v>
+      </c>
+      <c r="G59" s="16">
+        <v>0</v>
+      </c>
+      <c r="H59" s="16">
+        <v>0</v>
+      </c>
+      <c r="I59" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="6"/>
       <c r="K59" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3109,26 +3091,26 @@
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="46"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="47" t="s">
+      <c r="B60" s="18"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F60" s="41">
-        <v>0</v>
-      </c>
-      <c r="G60" s="41">
-        <v>0</v>
-      </c>
-      <c r="H60" s="41">
-        <v>0</v>
-      </c>
-      <c r="I60" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="7"/>
+      <c r="F60" s="16">
+        <v>0</v>
+      </c>
+      <c r="G60" s="16">
+        <v>0</v>
+      </c>
+      <c r="H60" s="16">
+        <v>0</v>
+      </c>
+      <c r="I60" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="6"/>
       <c r="K60" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3138,31 +3120,31 @@
         <v>.</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="50" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49"/>
-      <c r="B61" s="43" t="s">
+    <row r="61" spans="1:12" s="23" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22"/>
+      <c r="B61" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="41">
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="16">
         <f>SUM(F62:F64)</f>
         <v>0</v>
       </c>
-      <c r="G61" s="41">
-        <f t="shared" ref="G61:I61" si="8">SUM(G62:G64)</f>
-        <v>0</v>
-      </c>
-      <c r="H61" s="41">
+      <c r="G61" s="16">
+        <f t="shared" ref="G61:H61" si="8">SUM(G62:G64)</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I61" s="42">
+      <c r="I61" s="17">
         <f>SUM(I62:I64)</f>
         <v>0</v>
       </c>
-      <c r="J61" s="7"/>
+      <c r="J61" s="6"/>
       <c r="K61" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3172,31 +3154,31 @@
         <v>.</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49"/>
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
-      <c r="E62" s="53" t="s">
+    <row r="62" spans="1:12" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="22"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="41">
+      <c r="F62" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Juli",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$60)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="41">
+      <c r="G62" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Agustus",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$60)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="41">
+      <c r="H62" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"September",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$60)</f>
         <v>0</v>
       </c>
-      <c r="I62" s="54">
+      <c r="I62" s="27">
         <f>SUM(F62:H62)</f>
         <v>0</v>
       </c>
-      <c r="J62" s="7"/>
+      <c r="J62" s="6"/>
       <c r="K62" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3206,31 +3188,31 @@
         <v>.</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="53" t="s">
+    <row r="63" spans="1:12" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F63" s="41">
+      <c r="F63" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Juli",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$61)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="41">
+      <c r="G63" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Agustus",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$61)</f>
         <v>0</v>
       </c>
-      <c r="H63" s="41">
+      <c r="H63" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"September",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$61)</f>
         <v>0</v>
       </c>
-      <c r="I63" s="54">
+      <c r="I63" s="27">
         <f>SUM(F63:H63)</f>
         <v>0</v>
       </c>
-      <c r="J63" s="7"/>
+      <c r="J63" s="6"/>
       <c r="K63" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3240,31 +3222,31 @@
         <v>.</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49"/>
-      <c r="B64" s="51"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="52"/>
-      <c r="E64" s="53" t="s">
+    <row r="64" spans="1:12" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="F64" s="41">
+      <c r="F64" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Juli",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$62)</f>
         <v>0</v>
       </c>
-      <c r="G64" s="41">
+      <c r="G64" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Agustus",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$62)</f>
         <v>0</v>
       </c>
-      <c r="H64" s="41">
+      <c r="H64" s="16">
         <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"September",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$62)</f>
         <v>0</v>
       </c>
-      <c r="I64" s="54">
+      <c r="I64" s="27">
         <f>SUM(F64:H64)</f>
         <v>0</v>
       </c>
-      <c r="J64" s="7"/>
+      <c r="J64" s="6"/>
       <c r="K64" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3274,124 +3256,125 @@
         <v>.</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="50" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="49"/>
-      <c r="B65" s="55" t="s">
+    <row r="65" spans="1:10" s="23" customFormat="1" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="22"/>
+      <c r="B65" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="56"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="57">
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="40">
         <f>F6+F7-I8</f>
         <v>24290000</v>
       </c>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="59"/>
-      <c r="J65" s="60"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="42"/>
+      <c r="J65" s="28"/>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
-      <c r="J66" s="7"/>
+      <c r="J66" s="6"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
-      <c r="C67" s="61" t="s">
+      <c r="C67" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="J67" s="7"/>
+      <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
-      <c r="C68" s="61" t="s">
+      <c r="C68" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F68" s="62" t="s">
+      <c r="F68" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="62"/>
-      <c r="J68" s="7"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="43"/>
+      <c r="J68" s="6"/>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
-      <c r="C69" s="63"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="61"/>
-      <c r="H69" s="61"/>
-      <c r="I69" s="61"/>
-      <c r="J69" s="7"/>
+      <c r="C69" s="30"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="6"/>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
-      <c r="C70" s="63"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="61"/>
-      <c r="I70" s="61"/>
-      <c r="J70" s="7"/>
+      <c r="C70" s="30"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="6"/>
     </row>
     <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
-      <c r="C71" s="63"/>
-      <c r="F71" s="61"/>
-      <c r="G71" s="61"/>
-      <c r="H71" s="61"/>
-      <c r="I71" s="61"/>
-      <c r="J71" s="7"/>
+      <c r="C71" s="30"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="C72" s="64">
+      <c r="C72" s="31">
         <f>[1]REKAPITULASI!E50</f>
         <v>0</v>
       </c>
-      <c r="F72" s="65">
+      <c r="F72" s="44">
         <f>[1]REKAPITULASI!C9</f>
         <v>0</v>
       </c>
-      <c r="G72" s="65"/>
-      <c r="H72" s="65"/>
-      <c r="I72" s="65"/>
-      <c r="J72" s="7"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="44"/>
+      <c r="J72" s="6"/>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="C73" s="66" t="str">
+      <c r="C73" s="32" t="str">
         <f>[1]REKAPITULASI!E51</f>
         <v xml:space="preserve">NIP. </v>
       </c>
-      <c r="F73" s="67" t="str">
+      <c r="F73" s="45" t="str">
         <f>"NIP. "&amp;[1]REKAPITULASI!C10</f>
         <v xml:space="preserve">NIP. </v>
       </c>
-      <c r="G73" s="67"/>
-      <c r="H73" s="67"/>
-      <c r="I73" s="68"/>
-      <c r="J73" s="7"/>
+      <c r="G73" s="45"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="46"/>
+      <c r="J73" s="6"/>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="69"/>
-      <c r="B74" s="70"/>
-      <c r="C74" s="70"/>
-      <c r="D74" s="70"/>
-      <c r="E74" s="70"/>
-      <c r="F74" s="70"/>
-      <c r="G74" s="70"/>
-      <c r="H74" s="70"/>
-      <c r="I74" s="70"/>
-      <c r="J74" s="71"/>
+      <c r="A74" s="33"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
+      <c r="H74" s="34"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="35"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="18">
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
     <mergeCell ref="F73:I73"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="F7:I7"/>
@@ -3399,25 +3382,24 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F72:I72"/>
   </mergeCells>
   <conditionalFormatting sqref="L11:L12">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>L11="tidak satuan ratusan"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13:L14">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>L13="tidak satuan ratusan"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L29 L33:L64">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>L16="tidak satuan ratusan"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Laporan Belanja Modal Fix
Fix:
Laporan Belanja Modal

WIP:
Laporan K7 Provinsi
Laporan K7 Kabupaten
</commit_message>
<xml_diff>
--- a/format/k7_kab1.xlsx
+++ b/format/k7_kab1.xlsx
@@ -8,27 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\amanbos\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA39EE44-A064-4A9B-B68D-3DDED3F443FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78766FDB-A977-4869-B63C-FDAA1AAC80D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2806AC20-E28C-4D3D-8610-2A31688B425C}"/>
   </bookViews>
   <sheets>
     <sheet name="K7 TW 3 KAB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
+    <definedName name="bulan1">'K7 TW 3 KAB'!$F$9</definedName>
+    <definedName name="bulan2">'K7 TW 3 KAB'!$G$9</definedName>
+    <definedName name="bulan3">'K7 TW 3 KAB'!$H$9</definedName>
     <definedName name="judul">'K7 TW 3 KAB'!$B$2</definedName>
     <definedName name="nama_bendahara">'K7 TW 3 KAB'!$F$72</definedName>
     <definedName name="nama_kecamatan">'K7 TW 3 KAB'!$H$4</definedName>
     <definedName name="nama_kepsek">'K7 TW 3 KAB'!$C$72</definedName>
     <definedName name="nama_sekolah">'K7 TW 3 KAB'!$D$4</definedName>
+    <definedName name="nama_triwulan">'K7 TW 3 KAB'!$I$9</definedName>
     <definedName name="nip_bendahara">'K7 TW 3 KAB'!$F$73</definedName>
     <definedName name="nip_kepsek">'K7 TW 3 KAB'!$C$73</definedName>
     <definedName name="npsn">'K7 TW 3 KAB'!$B$4</definedName>
+    <definedName name="penerimaan_tw">'K7 TW 3 KAB'!$B$7</definedName>
     <definedName name="penerimaan_twsekarang">'K7 TW 3 KAB'!$F$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'K7 TW 3 KAB'!$A$1:$J$74</definedName>
+    <definedName name="saldo_tw">'K7 TW 3 KAB'!$B$6</definedName>
     <definedName name="saldo_twlalu">'K7 TW 3 KAB'!$F$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>REKAPITULASI PENGGUNAAN DANA BOS TRIWULAN 3 TAHUN 2019</t>
   </si>
@@ -247,6 +250,15 @@
   </si>
   <si>
     <t>Pemegang Kas Sekolah</t>
+  </si>
+  <si>
+    <t>SD NEGERI BATUR 01</t>
+  </si>
+  <si>
+    <t>GETASAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIP. </t>
   </si>
 </sst>
 </file>
@@ -784,7 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -828,9 +840,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
@@ -861,9 +870,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -891,6 +897,48 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -918,48 +966,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,6 +1004,18 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1037,92 +1055,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PETUNJUK"/>
-      <sheetName val="REKAPITULASI"/>
-      <sheetName val="BELANJA"/>
-      <sheetName val="CEK"/>
-      <sheetName val="LAP REALISASI"/>
-      <sheetName val="SPTJ"/>
-      <sheetName val="SPTMH"/>
-      <sheetName val="K7 TW 3 PROV"/>
-      <sheetName val="K7 TW 3 KAB"/>
-      <sheetName val="BELANJA MODAL"/>
-      <sheetName val="Persediaan"/>
-      <sheetName val="KET. BELANJA"/>
-      <sheetName val="data NPSN"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="B4">
-            <v>20320774</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>SD NEGERI BATUR 01</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>GETASAN</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51" t="str">
-            <v xml:space="preserve">NIP. </v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="60">
-          <cell r="R60" t="str">
-            <v>(3.01) Belanja Modal Mesin dan Peralatan</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="R61" t="str">
-            <v>(3.02) Belanja Modal Aset tetap Lainnya</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="R62" t="str">
-            <v>(3.03) Belanja Modal Gedung &amp; Bangunan</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="5">
-          <cell r="C5">
-            <v>11650000</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>12640000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1429,7 +1361,7 @@
   <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:I6"/>
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1369,7 @@
     <col min="1" max="1" width="4.77734375" style="4" customWidth="1"/>
     <col min="2" max="9" width="14.21875" style="4"/>
     <col min="10" max="10" width="4.77734375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="5" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0.44140625" style="4" customWidth="1"/>
     <col min="12" max="12" width="19.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="14.21875" style="4"/>
   </cols>
@@ -1456,16 +1388,16 @@
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
+      <c r="B2" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1474,23 +1406,20 @@
     </row>
     <row r="4" spans="1:12" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="60">
-        <f>[1]REKAPITULASI!B4</f>
+      <c r="B4" s="58">
         <v>20320774</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="62" t="str">
-        <f>[1]REKAPITULASI!C4</f>
-        <v>SD NEGERI BATUR 01</v>
-      </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65" t="str">
-        <f>[1]REKAPITULASI!F4</f>
-        <v>GETASAN</v>
-      </c>
-      <c r="I4" s="66"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="64"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1499,46 +1428,44 @@
     </row>
     <row r="6" spans="1:12" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69">
-        <f>[1]CEK!C5</f>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="67">
         <v>11650000</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="71"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="49">
-        <f>[1]CEK!C6</f>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38">
         <v>12640000</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="7">
         <f>F10+F15+F61</f>
         <v>0</v>
@@ -1559,10 +1486,10 @@
     </row>
     <row r="9" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="9" t="s">
         <v>4</v>
       </c>
@@ -1579,12 +1506,12 @@
     </row>
     <row r="10" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="11">
         <f>SUM(F11:F14)</f>
         <v>0</v>
@@ -1608,19 +1535,19 @@
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="16">
-        <v>0</v>
-      </c>
-      <c r="G11" s="16">
-        <v>0</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0</v>
-      </c>
-      <c r="I11" s="17">
+      <c r="F11" s="15">
+        <v>0</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16">
         <f>SUM(F11:H11)</f>
         <v>0</v>
       </c>
@@ -1639,25 +1566,25 @@
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="16">
-        <v>0</v>
-      </c>
-      <c r="G12" s="16">
-        <v>0</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="16">
         <f>SUM(F12:H12)</f>
         <v>0</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="4" t="str">
-        <f t="shared" ref="K12:K29" si="2">RIGHT(I12,2)</f>
+        <f t="shared" ref="K12:K32" si="2">RIGHT(I12,2)</f>
         <v>0</v>
       </c>
       <c r="L12" s="4" t="str">
@@ -1670,19 +1597,19 @@
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="16">
-        <v>0</v>
-      </c>
-      <c r="G13" s="16">
-        <v>0</v>
-      </c>
-      <c r="H13" s="16">
-        <v>0</v>
-      </c>
-      <c r="I13" s="17">
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0</v>
+      </c>
+      <c r="I13" s="16">
         <f>SUM(F13:H13)</f>
         <v>0</v>
       </c>
@@ -1692,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="4" t="str">
-        <f t="shared" ref="L13:L29" si="3">IF(OR(K13="0",K13="00"),".","tidak satuan ratusan")</f>
+        <f t="shared" ref="L13:L34" si="3">IF(OR(K13="0",K13="00"),".","tidak satuan ratusan")</f>
         <v>.</v>
       </c>
     </row>
@@ -1701,19 +1628,19 @@
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="16">
-        <v>0</v>
-      </c>
-      <c r="G14" s="16">
-        <v>0</v>
-      </c>
-      <c r="H14" s="16">
-        <v>0</v>
-      </c>
-      <c r="I14" s="17">
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
+      <c r="H14" s="15">
+        <v>0</v>
+      </c>
+      <c r="I14" s="16">
         <f>SUM(F14:H14)</f>
         <v>0</v>
       </c>
@@ -1729,12 +1656,12 @@
     </row>
     <row r="15" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
       <c r="F15" s="11">
         <f>SUM(F16:F60)</f>
         <v>0</v>
@@ -1752,25 +1679,33 @@
         <v>0</v>
       </c>
       <c r="J15" s="6"/>
+      <c r="K15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>.</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="16">
-        <v>0</v>
-      </c>
-      <c r="H16" s="16">
-        <v>0</v>
-      </c>
-      <c r="I16" s="17">
+      <c r="F16" s="15">
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
         <f t="shared" ref="I16:I60" si="5">SUM(F16:H16)</f>
         <v>0</v>
       </c>
@@ -1786,22 +1721,22 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="16">
-        <v>0</v>
-      </c>
-      <c r="G17" s="16">
-        <v>0</v>
-      </c>
-      <c r="H17" s="16">
-        <v>0</v>
-      </c>
-      <c r="I17" s="17">
+      <c r="F17" s="15">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0</v>
+      </c>
+      <c r="I17" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1817,22 +1752,22 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="16">
-        <v>0</v>
-      </c>
-      <c r="G18" s="16">
-        <v>0</v>
-      </c>
-      <c r="H18" s="16">
-        <v>0</v>
-      </c>
-      <c r="I18" s="17">
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="15">
+        <v>0</v>
+      </c>
+      <c r="I18" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1848,22 +1783,22 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="16">
-        <v>0</v>
-      </c>
-      <c r="H19" s="16">
-        <v>0</v>
-      </c>
-      <c r="I19" s="17">
+      <c r="F19" s="15">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0</v>
+      </c>
+      <c r="I19" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1879,22 +1814,22 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="16">
-        <v>0</v>
-      </c>
-      <c r="G20" s="16">
-        <v>0</v>
-      </c>
-      <c r="H20" s="16">
-        <v>0</v>
-      </c>
-      <c r="I20" s="17">
+      <c r="F20" s="15">
+        <v>0</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+      <c r="H20" s="15">
+        <v>0</v>
+      </c>
+      <c r="I20" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1910,22 +1845,22 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="16">
-        <v>0</v>
-      </c>
-      <c r="G21" s="16">
-        <v>0</v>
-      </c>
-      <c r="H21" s="16">
-        <v>0</v>
-      </c>
-      <c r="I21" s="17">
+      <c r="F21" s="15">
+        <v>0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+      <c r="H21" s="15">
+        <v>0</v>
+      </c>
+      <c r="I21" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1941,22 +1876,22 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="16">
-        <v>0</v>
-      </c>
-      <c r="G22" s="16">
-        <v>0</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0</v>
-      </c>
-      <c r="I22" s="17">
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1972,22 +1907,22 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="16">
-        <v>0</v>
-      </c>
-      <c r="G23" s="16">
-        <v>0</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0</v>
-      </c>
-      <c r="I23" s="17">
+      <c r="F23" s="15">
+        <v>0</v>
+      </c>
+      <c r="G23" s="15">
+        <v>0</v>
+      </c>
+      <c r="H23" s="15">
+        <v>0</v>
+      </c>
+      <c r="I23" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2003,22 +1938,22 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="16">
-        <v>0</v>
-      </c>
-      <c r="G24" s="16">
-        <v>0</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0</v>
-      </c>
-      <c r="I24" s="17">
+      <c r="F24" s="15">
+        <v>0</v>
+      </c>
+      <c r="G24" s="15">
+        <v>0</v>
+      </c>
+      <c r="H24" s="15">
+        <v>0</v>
+      </c>
+      <c r="I24" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2034,22 +1969,22 @@
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="20" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="16">
-        <v>0</v>
-      </c>
-      <c r="G25" s="16">
-        <v>0</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0</v>
-      </c>
-      <c r="I25" s="17">
+      <c r="F25" s="15">
+        <v>0</v>
+      </c>
+      <c r="G25" s="15">
+        <v>0</v>
+      </c>
+      <c r="H25" s="15">
+        <v>0</v>
+      </c>
+      <c r="I25" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2065,22 +2000,22 @@
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="16">
-        <v>0</v>
-      </c>
-      <c r="G26" s="16">
-        <v>0</v>
-      </c>
-      <c r="H26" s="16">
-        <v>0</v>
-      </c>
-      <c r="I26" s="17">
+      <c r="F26" s="15">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0</v>
+      </c>
+      <c r="I26" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2096,22 +2031,22 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="16">
-        <v>0</v>
-      </c>
-      <c r="G27" s="16">
-        <v>0</v>
-      </c>
-      <c r="H27" s="16">
-        <v>0</v>
-      </c>
-      <c r="I27" s="17">
+      <c r="F27" s="15">
+        <v>0</v>
+      </c>
+      <c r="G27" s="15">
+        <v>0</v>
+      </c>
+      <c r="H27" s="15">
+        <v>0</v>
+      </c>
+      <c r="I27" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2127,22 +2062,22 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="16">
-        <v>0</v>
-      </c>
-      <c r="G28" s="16">
-        <v>0</v>
-      </c>
-      <c r="H28" s="16">
-        <v>0</v>
-      </c>
-      <c r="I28" s="17">
+      <c r="F28" s="15">
+        <v>0</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
+      <c r="H28" s="15">
+        <v>0</v>
+      </c>
+      <c r="I28" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2158,22 +2093,22 @@
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="16">
-        <v>0</v>
-      </c>
-      <c r="G29" s="16">
-        <v>0</v>
-      </c>
-      <c r="H29" s="16">
-        <v>0</v>
-      </c>
-      <c r="I29" s="17">
+      <c r="F29" s="15">
+        <v>0</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15">
+        <v>0</v>
+      </c>
+      <c r="I29" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2189,91 +2124,115 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="16">
-        <v>0</v>
-      </c>
-      <c r="G30" s="16">
-        <v>0</v>
-      </c>
-      <c r="H30" s="16">
-        <v>0</v>
-      </c>
-      <c r="I30" s="17">
+      <c r="F30" s="15">
+        <v>0</v>
+      </c>
+      <c r="G30" s="15">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15">
+        <v>0</v>
+      </c>
+      <c r="I30" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J30" s="6"/>
+      <c r="K30" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>.</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="16">
-        <v>0</v>
-      </c>
-      <c r="G31" s="16">
-        <v>0</v>
-      </c>
-      <c r="H31" s="16">
-        <v>0</v>
-      </c>
-      <c r="I31" s="17">
+      <c r="F31" s="15">
+        <v>0</v>
+      </c>
+      <c r="G31" s="15">
+        <v>0</v>
+      </c>
+      <c r="H31" s="15">
+        <v>0</v>
+      </c>
+      <c r="I31" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J31" s="6"/>
+      <c r="K31" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>.</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="16">
-        <v>0</v>
-      </c>
-      <c r="G32" s="16">
-        <v>0</v>
-      </c>
-      <c r="H32" s="16">
-        <v>0</v>
-      </c>
-      <c r="I32" s="17">
+      <c r="F32" s="15">
+        <v>0</v>
+      </c>
+      <c r="G32" s="15">
+        <v>0</v>
+      </c>
+      <c r="H32" s="15">
+        <v>0</v>
+      </c>
+      <c r="I32" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J32" s="6"/>
+      <c r="K32" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>.</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20" t="s">
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="16">
-        <v>0</v>
-      </c>
-      <c r="G33" s="16">
-        <v>0</v>
-      </c>
-      <c r="H33" s="16">
-        <v>0</v>
-      </c>
-      <c r="I33" s="17">
+      <c r="F33" s="15">
+        <v>0</v>
+      </c>
+      <c r="G33" s="15">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15">
+        <v>0</v>
+      </c>
+      <c r="I33" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2283,28 +2242,28 @@
         <v>0</v>
       </c>
       <c r="L33" s="4" t="str">
-        <f t="shared" ref="L33:L64" si="7">IF(OR(K33="0",K33="00"),".","tidak satuan ratusan")</f>
+        <f t="shared" si="3"/>
         <v>.</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="16">
-        <v>0</v>
-      </c>
-      <c r="G34" s="16">
-        <v>0</v>
-      </c>
-      <c r="H34" s="16">
-        <v>0</v>
-      </c>
-      <c r="I34" s="17">
+      <c r="F34" s="15">
+        <v>0</v>
+      </c>
+      <c r="G34" s="15">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15">
+        <v>0</v>
+      </c>
+      <c r="I34" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2313,25 +2272,29 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="L34" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>.</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="20" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="16">
-        <v>0</v>
-      </c>
-      <c r="G35" s="16">
-        <v>0</v>
-      </c>
-      <c r="H35" s="16">
-        <v>0</v>
-      </c>
-      <c r="I35" s="17">
+      <c r="F35" s="15">
+        <v>0</v>
+      </c>
+      <c r="G35" s="15">
+        <v>0</v>
+      </c>
+      <c r="H35" s="15">
+        <v>0</v>
+      </c>
+      <c r="I35" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2341,28 +2304,28 @@
         <v>0</v>
       </c>
       <c r="L35" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="L33:L64" si="7">IF(OR(K35="0",K35="00"),".","tidak satuan ratusan")</f>
         <v>.</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="20" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="16">
-        <v>0</v>
-      </c>
-      <c r="G36" s="16">
-        <v>0</v>
-      </c>
-      <c r="H36" s="16">
-        <v>0</v>
-      </c>
-      <c r="I36" s="17">
+      <c r="F36" s="15">
+        <v>0</v>
+      </c>
+      <c r="G36" s="15">
+        <v>0</v>
+      </c>
+      <c r="H36" s="15">
+        <v>0</v>
+      </c>
+      <c r="I36" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2378,22 +2341,22 @@
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20" t="s">
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="16">
-        <v>0</v>
-      </c>
-      <c r="G37" s="16">
-        <v>0</v>
-      </c>
-      <c r="H37" s="16">
-        <v>0</v>
-      </c>
-      <c r="I37" s="17">
+      <c r="F37" s="15">
+        <v>0</v>
+      </c>
+      <c r="G37" s="15">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15">
+        <v>0</v>
+      </c>
+      <c r="I37" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2409,22 +2372,22 @@
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20" t="s">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="16">
-        <v>0</v>
-      </c>
-      <c r="G38" s="16">
-        <v>0</v>
-      </c>
-      <c r="H38" s="16">
-        <v>0</v>
-      </c>
-      <c r="I38" s="17">
+      <c r="F38" s="15">
+        <v>0</v>
+      </c>
+      <c r="G38" s="15">
+        <v>0</v>
+      </c>
+      <c r="H38" s="15">
+        <v>0</v>
+      </c>
+      <c r="I38" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2440,22 +2403,22 @@
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="20" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="16">
-        <v>0</v>
-      </c>
-      <c r="G39" s="16">
-        <v>0</v>
-      </c>
-      <c r="H39" s="16">
-        <v>0</v>
-      </c>
-      <c r="I39" s="17">
+      <c r="F39" s="15">
+        <v>0</v>
+      </c>
+      <c r="G39" s="15">
+        <v>0</v>
+      </c>
+      <c r="H39" s="15">
+        <v>0</v>
+      </c>
+      <c r="I39" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2471,22 +2434,22 @@
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="20" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="16">
-        <v>0</v>
-      </c>
-      <c r="G40" s="16">
-        <v>0</v>
-      </c>
-      <c r="H40" s="16">
-        <v>0</v>
-      </c>
-      <c r="I40" s="17">
+      <c r="F40" s="15">
+        <v>0</v>
+      </c>
+      <c r="G40" s="15">
+        <v>0</v>
+      </c>
+      <c r="H40" s="15">
+        <v>0</v>
+      </c>
+      <c r="I40" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2502,22 +2465,22 @@
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="16">
-        <v>0</v>
-      </c>
-      <c r="G41" s="16">
-        <v>0</v>
-      </c>
-      <c r="H41" s="16">
-        <v>0</v>
-      </c>
-      <c r="I41" s="17">
+      <c r="F41" s="15">
+        <v>0</v>
+      </c>
+      <c r="G41" s="15">
+        <v>0</v>
+      </c>
+      <c r="H41" s="15">
+        <v>0</v>
+      </c>
+      <c r="I41" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2533,22 +2496,22 @@
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20" t="s">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="16">
-        <v>0</v>
-      </c>
-      <c r="G42" s="16">
-        <v>0</v>
-      </c>
-      <c r="H42" s="16">
-        <v>0</v>
-      </c>
-      <c r="I42" s="17">
+      <c r="F42" s="15">
+        <v>0</v>
+      </c>
+      <c r="G42" s="15">
+        <v>0</v>
+      </c>
+      <c r="H42" s="15">
+        <v>0</v>
+      </c>
+      <c r="I42" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2564,22 +2527,22 @@
     </row>
     <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="16">
-        <v>0</v>
-      </c>
-      <c r="G43" s="16">
-        <v>0</v>
-      </c>
-      <c r="H43" s="16">
-        <v>0</v>
-      </c>
-      <c r="I43" s="17">
+      <c r="F43" s="15">
+        <v>0</v>
+      </c>
+      <c r="G43" s="15">
+        <v>0</v>
+      </c>
+      <c r="H43" s="15">
+        <v>0</v>
+      </c>
+      <c r="I43" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2595,22 +2558,22 @@
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="20" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="16">
-        <v>0</v>
-      </c>
-      <c r="G44" s="16">
-        <v>0</v>
-      </c>
-      <c r="H44" s="16">
-        <v>0</v>
-      </c>
-      <c r="I44" s="17">
+      <c r="F44" s="15">
+        <v>0</v>
+      </c>
+      <c r="G44" s="15">
+        <v>0</v>
+      </c>
+      <c r="H44" s="15">
+        <v>0</v>
+      </c>
+      <c r="I44" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2626,22 +2589,22 @@
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="20" t="s">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="16">
-        <v>0</v>
-      </c>
-      <c r="G45" s="16">
-        <v>0</v>
-      </c>
-      <c r="H45" s="16">
-        <v>0</v>
-      </c>
-      <c r="I45" s="17">
+      <c r="F45" s="15">
+        <v>0</v>
+      </c>
+      <c r="G45" s="15">
+        <v>0</v>
+      </c>
+      <c r="H45" s="15">
+        <v>0</v>
+      </c>
+      <c r="I45" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2657,22 +2620,22 @@
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="20" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="16">
-        <v>0</v>
-      </c>
-      <c r="G46" s="16">
-        <v>0</v>
-      </c>
-      <c r="H46" s="16">
-        <v>0</v>
-      </c>
-      <c r="I46" s="17">
+      <c r="F46" s="15">
+        <v>0</v>
+      </c>
+      <c r="G46" s="15">
+        <v>0</v>
+      </c>
+      <c r="H46" s="15">
+        <v>0</v>
+      </c>
+      <c r="I46" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2688,22 +2651,22 @@
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="20" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="16">
-        <v>0</v>
-      </c>
-      <c r="G47" s="16">
-        <v>0</v>
-      </c>
-      <c r="H47" s="16">
-        <v>0</v>
-      </c>
-      <c r="I47" s="17">
+      <c r="F47" s="15">
+        <v>0</v>
+      </c>
+      <c r="G47" s="15">
+        <v>0</v>
+      </c>
+      <c r="H47" s="15">
+        <v>0</v>
+      </c>
+      <c r="I47" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2719,22 +2682,22 @@
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="20" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="16">
-        <v>0</v>
-      </c>
-      <c r="G48" s="16">
-        <v>0</v>
-      </c>
-      <c r="H48" s="16">
-        <v>0</v>
-      </c>
-      <c r="I48" s="17">
+      <c r="F48" s="15">
+        <v>0</v>
+      </c>
+      <c r="G48" s="15">
+        <v>0</v>
+      </c>
+      <c r="H48" s="15">
+        <v>0</v>
+      </c>
+      <c r="I48" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2750,22 +2713,22 @@
     </row>
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="20" t="s">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F49" s="16">
-        <v>0</v>
-      </c>
-      <c r="G49" s="16">
-        <v>0</v>
-      </c>
-      <c r="H49" s="16">
-        <v>0</v>
-      </c>
-      <c r="I49" s="17">
+      <c r="F49" s="15">
+        <v>0</v>
+      </c>
+      <c r="G49" s="15">
+        <v>0</v>
+      </c>
+      <c r="H49" s="15">
+        <v>0</v>
+      </c>
+      <c r="I49" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2781,22 +2744,22 @@
     </row>
     <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="20" t="s">
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F50" s="16">
-        <v>0</v>
-      </c>
-      <c r="G50" s="16">
-        <v>0</v>
-      </c>
-      <c r="H50" s="16">
-        <v>0</v>
-      </c>
-      <c r="I50" s="17">
+      <c r="F50" s="15">
+        <v>0</v>
+      </c>
+      <c r="G50" s="15">
+        <v>0</v>
+      </c>
+      <c r="H50" s="15">
+        <v>0</v>
+      </c>
+      <c r="I50" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2812,22 +2775,22 @@
     </row>
     <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="20" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="16">
-        <v>0</v>
-      </c>
-      <c r="G51" s="16">
-        <v>0</v>
-      </c>
-      <c r="H51" s="16">
-        <v>0</v>
-      </c>
-      <c r="I51" s="17">
+      <c r="F51" s="15">
+        <v>0</v>
+      </c>
+      <c r="G51" s="15">
+        <v>0</v>
+      </c>
+      <c r="H51" s="15">
+        <v>0</v>
+      </c>
+      <c r="I51" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2843,22 +2806,22 @@
     </row>
     <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="20" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F52" s="16">
-        <v>0</v>
-      </c>
-      <c r="G52" s="16">
-        <v>0</v>
-      </c>
-      <c r="H52" s="16">
-        <v>0</v>
-      </c>
-      <c r="I52" s="17">
+      <c r="F52" s="15">
+        <v>0</v>
+      </c>
+      <c r="G52" s="15">
+        <v>0</v>
+      </c>
+      <c r="H52" s="15">
+        <v>0</v>
+      </c>
+      <c r="I52" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2874,22 +2837,22 @@
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="20" t="s">
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F53" s="16">
-        <v>0</v>
-      </c>
-      <c r="G53" s="16">
-        <v>0</v>
-      </c>
-      <c r="H53" s="16">
-        <v>0</v>
-      </c>
-      <c r="I53" s="17">
+      <c r="F53" s="15">
+        <v>0</v>
+      </c>
+      <c r="G53" s="15">
+        <v>0</v>
+      </c>
+      <c r="H53" s="15">
+        <v>0</v>
+      </c>
+      <c r="I53" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2905,22 +2868,22 @@
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="20" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="16">
-        <v>0</v>
-      </c>
-      <c r="G54" s="16">
-        <v>0</v>
-      </c>
-      <c r="H54" s="16">
-        <v>0</v>
-      </c>
-      <c r="I54" s="17">
+      <c r="F54" s="15">
+        <v>0</v>
+      </c>
+      <c r="G54" s="15">
+        <v>0</v>
+      </c>
+      <c r="H54" s="15">
+        <v>0</v>
+      </c>
+      <c r="I54" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2936,22 +2899,22 @@
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="20" t="s">
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="16">
-        <v>0</v>
-      </c>
-      <c r="G55" s="16">
-        <v>0</v>
-      </c>
-      <c r="H55" s="16">
-        <v>0</v>
-      </c>
-      <c r="I55" s="17">
+      <c r="F55" s="15">
+        <v>0</v>
+      </c>
+      <c r="G55" s="15">
+        <v>0</v>
+      </c>
+      <c r="H55" s="15">
+        <v>0</v>
+      </c>
+      <c r="I55" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2967,22 +2930,22 @@
     </row>
     <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="20" t="s">
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="16">
-        <v>0</v>
-      </c>
-      <c r="G56" s="16">
-        <v>0</v>
-      </c>
-      <c r="H56" s="16">
-        <v>0</v>
-      </c>
-      <c r="I56" s="17">
+      <c r="F56" s="15">
+        <v>0</v>
+      </c>
+      <c r="G56" s="15">
+        <v>0</v>
+      </c>
+      <c r="H56" s="15">
+        <v>0</v>
+      </c>
+      <c r="I56" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2998,22 +2961,22 @@
     </row>
     <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="20" t="s">
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F57" s="16">
-        <v>0</v>
-      </c>
-      <c r="G57" s="16">
-        <v>0</v>
-      </c>
-      <c r="H57" s="16">
-        <v>0</v>
-      </c>
-      <c r="I57" s="17">
+      <c r="F57" s="15">
+        <v>0</v>
+      </c>
+      <c r="G57" s="15">
+        <v>0</v>
+      </c>
+      <c r="H57" s="15">
+        <v>0</v>
+      </c>
+      <c r="I57" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3029,22 +2992,22 @@
     </row>
     <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="20" t="s">
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F58" s="16">
-        <v>0</v>
-      </c>
-      <c r="G58" s="16">
-        <v>0</v>
-      </c>
-      <c r="H58" s="16">
-        <v>0</v>
-      </c>
-      <c r="I58" s="17">
+      <c r="F58" s="15">
+        <v>0</v>
+      </c>
+      <c r="G58" s="15">
+        <v>0</v>
+      </c>
+      <c r="H58" s="15">
+        <v>0</v>
+      </c>
+      <c r="I58" s="16">
         <f>SUM(F58:H58)</f>
         <v>0</v>
       </c>
@@ -3060,22 +3023,22 @@
     </row>
     <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="20" t="s">
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F59" s="16">
-        <v>0</v>
-      </c>
-      <c r="G59" s="16">
-        <v>0</v>
-      </c>
-      <c r="H59" s="16">
-        <v>0</v>
-      </c>
-      <c r="I59" s="17">
+      <c r="F59" s="15">
+        <v>0</v>
+      </c>
+      <c r="G59" s="15">
+        <v>0</v>
+      </c>
+      <c r="H59" s="15">
+        <v>0</v>
+      </c>
+      <c r="I59" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3091,22 +3054,22 @@
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="20" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F60" s="16">
-        <v>0</v>
-      </c>
-      <c r="G60" s="16">
-        <v>0</v>
-      </c>
-      <c r="H60" s="16">
-        <v>0</v>
-      </c>
-      <c r="I60" s="17">
+      <c r="F60" s="15">
+        <v>0</v>
+      </c>
+      <c r="G60" s="15">
+        <v>0</v>
+      </c>
+      <c r="H60" s="15">
+        <v>0</v>
+      </c>
+      <c r="I60" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3120,27 +3083,27 @@
         <v>.</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="23" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="36" t="s">
+    <row r="61" spans="1:12" s="22" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="16">
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="72">
         <f>SUM(F62:F64)</f>
         <v>0</v>
       </c>
-      <c r="G61" s="16">
+      <c r="G61" s="72">
         <f t="shared" ref="G61:H61" si="8">SUM(G62:G64)</f>
         <v>0</v>
       </c>
-      <c r="H61" s="16">
+      <c r="H61" s="72">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I61" s="17">
+      <c r="I61" s="73">
         <f>SUM(I62:I64)</f>
         <v>0</v>
       </c>
@@ -3154,27 +3117,24 @@
         <v>.</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="26" t="s">
+    <row r="62" spans="1:12" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Juli",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$60)</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Agustus",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$60)</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"September",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$60)</f>
-        <v>0</v>
-      </c>
-      <c r="I62" s="27">
+      <c r="F62" s="15">
+        <v>0</v>
+      </c>
+      <c r="G62" s="15">
+        <v>0</v>
+      </c>
+      <c r="H62" s="15">
+        <v>0</v>
+      </c>
+      <c r="I62" s="25">
         <f>SUM(F62:H62)</f>
         <v>0</v>
       </c>
@@ -3188,27 +3148,24 @@
         <v>.</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="26" t="s">
+    <row r="63" spans="1:12" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="F63" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Juli",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$61)</f>
-        <v>0</v>
-      </c>
-      <c r="G63" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Agustus",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$61)</f>
-        <v>0</v>
-      </c>
-      <c r="H63" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"September",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$61)</f>
-        <v>0</v>
-      </c>
-      <c r="I63" s="27">
+      <c r="F63" s="15">
+        <v>0</v>
+      </c>
+      <c r="G63" s="15">
+        <v>0</v>
+      </c>
+      <c r="H63" s="15">
+        <v>0</v>
+      </c>
+      <c r="I63" s="25">
         <f>SUM(F63:H63)</f>
         <v>0</v>
       </c>
@@ -3222,27 +3179,24 @@
         <v>.</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="26" t="s">
+    <row r="64" spans="1:12" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F64" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Juli",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$62)</f>
-        <v>0</v>
-      </c>
-      <c r="G64" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"Agustus",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$62)</f>
-        <v>0</v>
-      </c>
-      <c r="H64" s="16">
-        <f>SUMIFS([1]BELANJA!$E$11:$E$1010,[1]BELANJA!$C$11:$C$1010,"September",[1]BELANJA!$H$11:$H$1010,[1]BELANJA!$R$62)</f>
-        <v>0</v>
-      </c>
-      <c r="I64" s="27">
+      <c r="F64" s="15">
+        <v>0</v>
+      </c>
+      <c r="G64" s="15">
+        <v>0</v>
+      </c>
+      <c r="H64" s="15">
+        <v>0</v>
+      </c>
+      <c r="I64" s="25">
         <f>SUM(F64:H64)</f>
         <v>0</v>
       </c>
@@ -3256,22 +3210,22 @@
         <v>.</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="23" customFormat="1" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="22"/>
-      <c r="B65" s="38" t="s">
+    <row r="65" spans="1:10" s="22" customFormat="1" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="21"/>
+      <c r="B65" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="40">
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="52">
         <f>F6+F7-I8</f>
         <v>24290000</v>
       </c>
-      <c r="G65" s="41"/>
-      <c r="H65" s="41"/>
-      <c r="I65" s="42"/>
-      <c r="J65" s="28"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="54"/>
+      <c r="J65" s="26"/>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
@@ -3279,92 +3233,88 @@
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="27" t="s">
         <v>64</v>
       </c>
       <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="F68" s="43" t="s">
+      <c r="F68" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="43"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
       <c r="J68" s="6"/>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
-      <c r="C69" s="30"/>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="29"/>
-      <c r="I69" s="29"/>
+      <c r="C69" s="28"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="27"/>
+      <c r="I69" s="27"/>
       <c r="J69" s="6"/>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
-      <c r="C70" s="30"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="29"/>
+      <c r="C70" s="28"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="27"/>
       <c r="J70" s="6"/>
     </row>
     <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
-      <c r="C71" s="30"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
+      <c r="C71" s="28"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="I71" s="27"/>
       <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="C72" s="31">
-        <f>[1]REKAPITULASI!E50</f>
-        <v>0</v>
-      </c>
-      <c r="F72" s="44">
-        <f>[1]REKAPITULASI!C9</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="44"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="44"/>
+      <c r="C72" s="29">
+        <v>0</v>
+      </c>
+      <c r="F72" s="56">
+        <v>0</v>
+      </c>
+      <c r="G72" s="56"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="56"/>
       <c r="J72" s="6"/>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="C73" s="32" t="str">
-        <f>[1]REKAPITULASI!E51</f>
-        <v xml:space="preserve">NIP. </v>
-      </c>
-      <c r="F73" s="45" t="str">
-        <f>"NIP. "&amp;[1]REKAPITULASI!C10</f>
-        <v xml:space="preserve">NIP. </v>
-      </c>
-      <c r="G73" s="45"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="46"/>
+      <c r="C73" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F73" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G73" s="34"/>
+      <c r="H73" s="34"/>
+      <c r="I73" s="35"/>
       <c r="J73" s="6"/>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="33"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="35"/>
+      <c r="A74" s="31"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="33"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -3393,12 +3343,12 @@
       <formula>L11="tidak satuan ratusan"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13:L14">
+  <conditionalFormatting sqref="L13:L15">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>L13="tidak satuan ratusan"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16:L29 L33:L64">
+  <conditionalFormatting sqref="L16:L64">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>L16="tidak satuan ratusan"</formula>
     </cfRule>

</xml_diff>